<commit_message>
antes de mudar entrada de dados
</commit_message>
<xml_diff>
--- a/profit/arquivos/asin.xlsx
+++ b/profit/arquivos/asin.xlsx
@@ -14,474 +14,336 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>ASIN</t>
   </si>
   <si>
-    <t>B005MI6BC6</t>
-  </si>
-  <si>
-    <t>B07DQSJ744</t>
-  </si>
-  <si>
-    <t>B008MDXKOU</t>
-  </si>
-  <si>
-    <t>B09SJ3DQFC</t>
-  </si>
-  <si>
-    <t>B012D6Q42Q</t>
-  </si>
-  <si>
-    <t>B098QZVQKL</t>
-  </si>
-  <si>
-    <t>B00UMCBLS6</t>
-  </si>
-  <si>
-    <t>B0CZ7JFP4C</t>
-  </si>
-  <si>
-    <t>B084KL5JYK</t>
-  </si>
-  <si>
-    <t>B0CZBZQWCS</t>
-  </si>
-  <si>
-    <t>B00TI4HL8S</t>
-  </si>
-  <si>
-    <t>B012YDYEDY</t>
-  </si>
-  <si>
-    <t>B077K83183</t>
-  </si>
-  <si>
-    <t>B09JB99R9G</t>
-  </si>
-  <si>
-    <t>B09YFFPVB2</t>
-  </si>
-  <si>
-    <t>B0115GWOOC</t>
-  </si>
-  <si>
-    <t>B07WGF6J3P</t>
-  </si>
-  <si>
-    <t>B09VHBRKT9</t>
-  </si>
-  <si>
-    <t>B01N9XQ7NK</t>
-  </si>
-  <si>
-    <t>B088WY54ZH</t>
-  </si>
-  <si>
-    <t>B088NQRD19</t>
-  </si>
-  <si>
-    <t>B008MDPFEI</t>
-  </si>
-  <si>
-    <t>B09WBVDJPX</t>
-  </si>
-  <si>
-    <t>B095XF97ZK</t>
-  </si>
-  <si>
-    <t>B09KMC67Q9</t>
-  </si>
-  <si>
-    <t>B09SMXPMZJ</t>
-  </si>
-  <si>
-    <t>B00UIR2AGC</t>
-  </si>
-  <si>
-    <t>B018WNUF3S</t>
-  </si>
-  <si>
-    <t>B098KGJYTR</t>
-  </si>
-  <si>
-    <t>B09X1Y4HV6</t>
-  </si>
-  <si>
-    <t>B0C7RNY3GW</t>
-  </si>
-  <si>
-    <t>B0137IR0H2</t>
-  </si>
-  <si>
-    <t>B01JT0FA9W</t>
-  </si>
-  <si>
-    <t>B08TT1SZPC</t>
-  </si>
-  <si>
-    <t>B09JBC698R</t>
-  </si>
-  <si>
-    <t>B09H6XS3GR</t>
-  </si>
-  <si>
-    <t>B005T90QGK</t>
-  </si>
-  <si>
-    <t>B007M7PUR2</t>
-  </si>
-  <si>
-    <t>B0843K2XZ3</t>
-  </si>
-  <si>
-    <t>B018CPQFE4</t>
-  </si>
-  <si>
-    <t>B00MEJ972W</t>
-  </si>
-  <si>
-    <t>B0813QWBWY</t>
-  </si>
-  <si>
-    <t>B005TBCXUK</t>
-  </si>
-  <si>
-    <t>B09TD2G26P</t>
-  </si>
-  <si>
-    <t>B09X63TQ8Q</t>
-  </si>
-  <si>
-    <t>B09XN7MD56</t>
-  </si>
-  <si>
-    <t>B00AAGJBFO</t>
-  </si>
-  <si>
-    <t>B00FRBYJI6</t>
-  </si>
-  <si>
-    <t>B09LPML4DZ</t>
-  </si>
-  <si>
-    <t>B088TQYQWG</t>
-  </si>
-  <si>
-    <t>B006Z10DD2</t>
-  </si>
-  <si>
-    <t>B009NAK44U</t>
-  </si>
-  <si>
-    <t>B08R8ZCSW6</t>
-  </si>
-  <si>
-    <t>B00KV51DTQ</t>
-  </si>
-  <si>
-    <t>B081RYHCRT</t>
-  </si>
-  <si>
-    <t>B081RY2XLC</t>
-  </si>
-  <si>
-    <t>B088WWZZFF</t>
-  </si>
-  <si>
-    <t>B07CT5MG4G</t>
-  </si>
-  <si>
-    <t>B00V3L522G</t>
-  </si>
-  <si>
-    <t>B01DL6UAIQ</t>
-  </si>
-  <si>
-    <t>B071WXF3LW</t>
-  </si>
-  <si>
-    <t>B079PB9T7Y</t>
-  </si>
-  <si>
-    <t>B00BC94536</t>
-  </si>
-  <si>
-    <t>B00Q7VQGF4</t>
-  </si>
-  <si>
-    <t>B088NKGD44</t>
-  </si>
-  <si>
-    <t>B016YWZCD2</t>
-  </si>
-  <si>
-    <t>B01JGMRN66</t>
-  </si>
-  <si>
-    <t>B0B8K1FXXW</t>
-  </si>
-  <si>
-    <t>B08VCYY6QN</t>
-  </si>
-  <si>
-    <t>B005T7O9VA</t>
-  </si>
-  <si>
-    <t>B01GBJR4G6</t>
-  </si>
-  <si>
-    <t>B093PBVJ74</t>
-  </si>
-  <si>
-    <t>B00KSS1TYU</t>
-  </si>
-  <si>
-    <t>B00KSNPU1I</t>
-  </si>
-  <si>
-    <t>B010IILDQ8</t>
-  </si>
-  <si>
-    <t>B010IJ0WLE</t>
-  </si>
-  <si>
-    <t>B005T94J54</t>
-  </si>
-  <si>
-    <t>B00KSL3L3E</t>
-  </si>
-  <si>
-    <t>B00KSGPP38</t>
-  </si>
-  <si>
-    <t>B00KI6GUIM</t>
-  </si>
-  <si>
-    <t>B00KI5XB08</t>
-  </si>
-  <si>
-    <t>B011OP0BKI</t>
-  </si>
-  <si>
-    <t>B00MEJOLR8</t>
-  </si>
-  <si>
-    <t>B011ORX554</t>
-  </si>
-  <si>
-    <t>B005S41H2S</t>
-  </si>
-  <si>
-    <t>B0084ZUABC</t>
-  </si>
-  <si>
-    <t>B09TG2NH1Q</t>
-  </si>
-  <si>
-    <t>B00KSLDU6W</t>
-  </si>
-  <si>
-    <t>B0BGRKG1TN</t>
-  </si>
-  <si>
-    <t>B09CYMJ177</t>
-  </si>
-  <si>
-    <t>B0BXZ5LCVR</t>
-  </si>
-  <si>
-    <t>B09WZPX6MM</t>
-  </si>
-  <si>
-    <t>B07SS6QF52</t>
-  </si>
-  <si>
-    <t>B07NVYJML4</t>
-  </si>
-  <si>
-    <t>B00X95300U</t>
-  </si>
-  <si>
-    <t>B01N5VUQPT</t>
-  </si>
-  <si>
-    <t>B00B7Z7FNM</t>
-  </si>
-  <si>
-    <t>B011OYOZ7E</t>
-  </si>
-  <si>
-    <t>B00U7W88XM</t>
-  </si>
-  <si>
-    <t>B07JJ1TD6R</t>
-  </si>
-  <si>
-    <t>B01GDRE9MI</t>
-  </si>
-  <si>
-    <t>B011ONMMUM</t>
-  </si>
-  <si>
-    <t>B07WV62KW5</t>
-  </si>
-  <si>
-    <t>B00TT6W036</t>
-  </si>
-  <si>
-    <t>B00TT6W09A</t>
-  </si>
-  <si>
-    <t>B01F4KF1FO</t>
-  </si>
-  <si>
-    <t>B005T5CIY2</t>
-  </si>
-  <si>
-    <t>B000LE6ZF4</t>
-  </si>
-  <si>
-    <t>B076LN245W</t>
-  </si>
-  <si>
-    <t>B00DLSKIXW</t>
-  </si>
-  <si>
-    <t>B003UQV1JK</t>
-  </si>
-  <si>
-    <t>B00CONDW92</t>
-  </si>
-  <si>
-    <t>B0D372YKQR</t>
-  </si>
-  <si>
-    <t>B00MEJDAGQ</t>
+    <t>B004YXWOI0</t>
+  </si>
+  <si>
+    <t>B000UWCQJ6</t>
+  </si>
+  <si>
+    <t>B0091WERKW</t>
+  </si>
+  <si>
+    <t>B07RY7JM6Z</t>
+  </si>
+  <si>
+    <t>B0018L982G</t>
+  </si>
+  <si>
+    <t>B004V3JK3A</t>
+  </si>
+  <si>
+    <t>B004YXW3U4</t>
+  </si>
+  <si>
+    <t>B004YXVLB6</t>
+  </si>
+  <si>
+    <t>B07FBS8T45</t>
+  </si>
+  <si>
+    <t>B07H8Q1FBV</t>
+  </si>
+  <si>
+    <t>982071978X</t>
+  </si>
+  <si>
+    <t>B07SFW51YQ</t>
+  </si>
+  <si>
+    <t>B000ONRFKQ</t>
+  </si>
+  <si>
+    <t>B07FBVPCZ3</t>
+  </si>
+  <si>
+    <t>B003U65C9A</t>
+  </si>
+  <si>
+    <t>B0091WHXDU</t>
+  </si>
+  <si>
+    <t>9820794587</t>
+  </si>
+  <si>
+    <t>B011ONBQ7C</t>
+  </si>
+  <si>
+    <t>B00CONH4AU</t>
+  </si>
+  <si>
+    <t>B00NGX1HZK</t>
+  </si>
+  <si>
+    <t>B002QHYKNS</t>
+  </si>
+  <si>
+    <t>B001NJKYLW</t>
+  </si>
+  <si>
+    <t>B007ID6704</t>
+  </si>
+  <si>
+    <t>B0741MYGYY</t>
+  </si>
+  <si>
+    <t>B001ZTMTKO</t>
+  </si>
+  <si>
+    <t>B000WL4GFM</t>
+  </si>
+  <si>
+    <t>B001ZRTS8W</t>
+  </si>
+  <si>
+    <t>B001ZTRYEK</t>
+  </si>
+  <si>
+    <t>B010SHKN2O</t>
+  </si>
+  <si>
+    <t>B001ZSBNH0</t>
+  </si>
+  <si>
+    <t>B0018L1MSO</t>
+  </si>
+  <si>
+    <t>B00CONLIKC</t>
+  </si>
+  <si>
+    <t>B000WLA4HQ</t>
   </si>
   <si>
     <t>B01I8Y3ZIS</t>
   </si>
   <si>
+    <t>B00DKYO8NS</t>
+  </si>
+  <si>
+    <t>B00CONDFWQ</t>
+  </si>
+  <si>
+    <t>B01KQQ5SUY</t>
+  </si>
+  <si>
+    <t>B001ZTKQ54</t>
+  </si>
+  <si>
+    <t>B018CR0NN6</t>
+  </si>
+  <si>
+    <t>B000WKXMUS</t>
+  </si>
+  <si>
+    <t>B001BAHOHU</t>
+  </si>
+  <si>
+    <t>B005CTIGK0</t>
+  </si>
+  <si>
+    <t>B00CONDN7I</t>
+  </si>
+  <si>
+    <t>B01BRS9VR6</t>
+  </si>
+  <si>
+    <t>B00CONOFA2</t>
+  </si>
+  <si>
+    <t>B0078S7S1Q</t>
+  </si>
+  <si>
+    <t>B00DBSTR3Y</t>
+  </si>
+  <si>
+    <t>B008KNW8YK</t>
+  </si>
+  <si>
+    <t>B0CWL9DYFQ</t>
+  </si>
+  <si>
+    <t>B000WL4VZ2</t>
+  </si>
+  <si>
+    <t>B007KHNZJ4</t>
+  </si>
+  <si>
+    <t>B0CWLFBLYP</t>
+  </si>
+  <si>
+    <t>B0078S0XX6</t>
+  </si>
+  <si>
+    <t>B001ZS1PA0</t>
+  </si>
+  <si>
+    <t>B008KNCY9O</t>
+  </si>
+  <si>
+    <t>B0018L593S</t>
+  </si>
+  <si>
+    <t>B0078S7W1C</t>
+  </si>
+  <si>
+    <t>B001ZPGXFK</t>
+  </si>
+  <si>
+    <t>B00CONK2YA</t>
+  </si>
+  <si>
+    <t>B07PKJBTP8</t>
+  </si>
+  <si>
+    <t>B00CONLBNG</t>
+  </si>
+  <si>
+    <t>B00CONDIM8</t>
+  </si>
+  <si>
+    <t>B001ZRKTKS</t>
+  </si>
+  <si>
+    <t>B00CONA286</t>
+  </si>
+  <si>
+    <t>B00E7BVWYQ</t>
+  </si>
+  <si>
+    <t>B0078RZ2ZG</t>
+  </si>
+  <si>
+    <t>B000WLA4XA</t>
+  </si>
+  <si>
+    <t>B00CONHZG8</t>
+  </si>
+  <si>
+    <t>B003APXFA4</t>
+  </si>
+  <si>
     <t>B00CONOB8I</t>
   </si>
   <si>
-    <t>B011OX734M</t>
-  </si>
-  <si>
-    <t>B07JFXZNLN</t>
-  </si>
-  <si>
-    <t>B001ZG935G</t>
-  </si>
-  <si>
-    <t>B01BKA5NBO</t>
-  </si>
-  <si>
-    <t>B00GQQTHCO</t>
-  </si>
-  <si>
-    <t>B07PW4N4R7</t>
-  </si>
-  <si>
-    <t>B0137I8BD4</t>
-  </si>
-  <si>
-    <t>B01N4EL07S</t>
-  </si>
-  <si>
-    <t>B08R595WNJ</t>
-  </si>
-  <si>
-    <t>B07CKWR5YD</t>
-  </si>
-  <si>
-    <t>B07LGDTLTT</t>
-  </si>
-  <si>
-    <t>B07LGFLZ57</t>
-  </si>
-  <si>
-    <t>B00YZ31YQM</t>
-  </si>
-  <si>
-    <t>9820631297</t>
-  </si>
-  <si>
-    <t>B07D6V76JN</t>
-  </si>
-  <si>
-    <t>B07D6VPNZF</t>
-  </si>
-  <si>
-    <t>B0151NHS1Y</t>
-  </si>
-  <si>
-    <t>B07LGFZPGT</t>
-  </si>
-  <si>
-    <t>B07PXTJ2CR</t>
-  </si>
-  <si>
-    <t>B07LGFKHVZ</t>
-  </si>
-  <si>
-    <t>B07LGD6KY1</t>
-  </si>
-  <si>
-    <t>B07LGF5DZ4</t>
-  </si>
-  <si>
-    <t>B07LGDVQJD</t>
-  </si>
-  <si>
-    <t>B0825DM3LH</t>
-  </si>
-  <si>
-    <t>B096G9YTX8</t>
-  </si>
-  <si>
-    <t>B07JL33QR9</t>
-  </si>
-  <si>
-    <t>B07LGG5X45</t>
-  </si>
-  <si>
-    <t>B07LGFQ857</t>
-  </si>
-  <si>
-    <t>B07RG5XH76</t>
-  </si>
-  <si>
-    <t>B071P418HJ</t>
-  </si>
-  <si>
-    <t>B005T9KMXW</t>
-  </si>
-  <si>
-    <t>B016YYY7WM</t>
-  </si>
-  <si>
-    <t>B005T5BQCM</t>
-  </si>
-  <si>
-    <t>B005S3QWLA</t>
-  </si>
-  <si>
-    <t>B07RH8QV4Z</t>
-  </si>
-  <si>
-    <t>B07RH8WM9M</t>
-  </si>
-  <si>
-    <t>B081NS27NX</t>
-  </si>
-  <si>
-    <t>B005T8K0TE</t>
-  </si>
-  <si>
-    <t>B09NS48TK</t>
+    <t>B0CWLCRC1C</t>
+  </si>
+  <si>
+    <t>B007EX91QA</t>
+  </si>
+  <si>
+    <t>B01G51TB48</t>
+  </si>
+  <si>
+    <t>B09J1JW9XW</t>
+  </si>
+  <si>
+    <t>B00CONPRWC</t>
+  </si>
+  <si>
+    <t>B00MEIH3S8</t>
+  </si>
+  <si>
+    <t>B0CWLB5DC5</t>
+  </si>
+  <si>
+    <t>B007IA4CW2</t>
+  </si>
+  <si>
+    <t>B07PZC78N4</t>
+  </si>
+  <si>
+    <t>B011OOMJ9U</t>
+  </si>
+  <si>
+    <t>B084J61V64</t>
+  </si>
+  <si>
+    <t>B011OP2D90</t>
+  </si>
+  <si>
+    <t>B000WL7PB4</t>
+  </si>
+  <si>
+    <t>B0028YOWU0</t>
+  </si>
+  <si>
+    <t>B01GA40UT0</t>
+  </si>
+  <si>
+    <t>B0831QZ1GJ</t>
+  </si>
+  <si>
+    <t>B07N7WC47S</t>
+  </si>
+  <si>
+    <t>B0080KNWZW</t>
+  </si>
+  <si>
+    <t>B01J24PH70</t>
+  </si>
+  <si>
+    <t>B001BDG13A</t>
+  </si>
+  <si>
+    <t>B07DVR8N1H</t>
+  </si>
+  <si>
+    <t>B003X2CT2Y</t>
+  </si>
+  <si>
+    <t>B00B7ZPXPE</t>
+  </si>
+  <si>
+    <t>B07GFNWYGC</t>
+  </si>
+  <si>
+    <t>B003U666EU</t>
+  </si>
+  <si>
+    <t>B07W6MCL6Z</t>
+  </si>
+  <si>
+    <t>B07FBWLB1F</t>
+  </si>
+  <si>
+    <t>B0091WI0UK</t>
+  </si>
+  <si>
+    <t>B07FBT44LM</t>
+  </si>
+  <si>
+    <t>B007KHZNIK</t>
+  </si>
+  <si>
+    <t>B001BDG18K</t>
+  </si>
+  <si>
+    <t>B001UHBQVO</t>
+  </si>
+  <si>
+    <t>B087X9JZBY</t>
+  </si>
+  <si>
+    <t>B07G2PPDBJ</t>
+  </si>
+  <si>
+    <t>B0018LBTGY</t>
+  </si>
+  <si>
+    <t>B0028YIWO2</t>
+  </si>
+  <si>
+    <t>B0020R12AI</t>
+  </si>
+  <si>
+    <t>B001ZRKS6I</t>
+  </si>
+  <si>
+    <t>B07X4879P</t>
   </si>
 </sst>
 </file>
@@ -853,16 +715,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A156"/>
+  <dimension ref="A1:A110"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1410,236 +1272,6 @@
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25">
       <c r="A110" s="2" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25">
-      <c r="A111" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="17.25">
-      <c r="A112" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="17.25">
-      <c r="A113" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="17.25">
-      <c r="A114" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="17.25">
-      <c r="A115" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="17.25">
-      <c r="A116" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="17.25">
-      <c r="A117" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="17.25">
-      <c r="A118" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="17.25">
-      <c r="A119" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="17.25">
-      <c r="A120" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="17.25">
-      <c r="A121" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="17.25">
-      <c r="A122" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="17.25">
-      <c r="A123" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="17.25">
-      <c r="A124" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="17.25">
-      <c r="A125" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="17.25">
-      <c r="A126" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="17.25">
-      <c r="A127" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="17.25">
-      <c r="A128" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="17.25">
-      <c r="A129" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="17.25">
-      <c r="A130" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="17.25">
-      <c r="A131" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="17.25">
-      <c r="A132" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="17.25">
-      <c r="A133" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="17.25">
-      <c r="A134" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="17.25">
-      <c r="A135" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="17.25">
-      <c r="A136" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="17.25">
-      <c r="A137" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="17.25">
-      <c r="A138" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="17.25">
-      <c r="A139" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="17.25">
-      <c r="A140" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="17.25">
-      <c r="A141" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="17.25">
-      <c r="A142" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="17.25">
-      <c r="A143" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="17.25">
-      <c r="A144" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="17.25">
-      <c r="A145" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="17.25">
-      <c r="A146" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="17.25">
-      <c r="A147" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="17.25">
-      <c r="A148" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="17.25">
-      <c r="A149" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="17.25">
-      <c r="A150" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="17.25">
-      <c r="A151" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="17.25">
-      <c r="A152" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="17.25">
-      <c r="A153" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="17.25">
-      <c r="A154" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="17.25">
-      <c r="A155" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="17.25">
-      <c r="A156" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>